<commit_message>
Add new mock data
</commit_message>
<xml_diff>
--- a/data/MockData.xlsx
+++ b/data/MockData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6324" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6324" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="7" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Peremptory_original" sheetId="6" r:id="rId4"/>
     <sheet name="Peremptory_modified" sheetId="4" r:id="rId5"/>
     <sheet name="Template" sheetId="3" r:id="rId6"/>
+    <sheet name="CourtB-Filing" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5007" uniqueCount="2405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5045" uniqueCount="2405">
   <si>
     <t>Case Type</t>
   </si>
@@ -7599,7 +7600,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -7845,13 +7846,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8039,6 +8051,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -8050,6 +8065,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -8626,7 +8647,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection sqref="A1:O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8637,24 +8658,24 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="75">
+      <c r="B1" s="76">
         <v>2016</v>
       </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="75">
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="76">
         <v>2017</v>
       </c>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="73" t="s">
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="74" t="s">
         <v>76</v>
       </c>
     </row>
@@ -8701,7 +8722,7 @@
       <c r="N2" s="69" t="s">
         <v>2367</v>
       </c>
-      <c r="O2" s="74"/>
+      <c r="O2" s="75"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -37068,9 +37089,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -37228,7 +37249,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="55">
-        <v>1.9</v>
+        <v>4</v>
       </c>
       <c r="E9" s="40"/>
       <c r="F9" s="47">
@@ -37236,12 +37257,12 @@
       </c>
       <c r="G9" s="48">
         <f t="shared" ref="G9:G15" si="2">D9/F9</f>
-        <v>2.3749999999999996</v>
+        <v>5</v>
       </c>
       <c r="H9" s="34"/>
       <c r="I9" s="33">
         <f>F9*G9</f>
-        <v>1.8999999999999997</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -37253,7 +37274,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="56">
-        <v>0.7</v>
+        <v>10</v>
       </c>
       <c r="E10" s="40"/>
       <c r="F10" s="49">
@@ -37261,12 +37282,12 @@
       </c>
       <c r="G10" s="48">
         <f t="shared" si="2"/>
-        <v>1.4</v>
+        <v>20</v>
       </c>
       <c r="H10" s="31"/>
       <c r="I10" s="33">
         <f t="shared" ref="I10:I15" si="3">F10*G10</f>
-        <v>0.7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -37328,7 +37349,7 @@
         <v>21</v>
       </c>
       <c r="D13" s="56">
-        <v>0.5</v>
+        <v>6</v>
       </c>
       <c r="E13" s="40"/>
       <c r="F13" s="49">
@@ -37336,12 +37357,12 @@
       </c>
       <c r="G13" s="48">
         <f t="shared" si="2"/>
-        <v>0.83333333333333337</v>
+        <v>10</v>
       </c>
       <c r="H13" s="31"/>
       <c r="I13" s="33">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -37353,7 +37374,7 @@
         <v>2388</v>
       </c>
       <c r="D14" s="56">
-        <v>0.8</v>
+        <v>3</v>
       </c>
       <c r="E14" s="40"/>
       <c r="F14" s="49">
@@ -37361,12 +37382,12 @@
       </c>
       <c r="G14" s="48">
         <f t="shared" si="2"/>
-        <v>1.3333333333333335</v>
+        <v>5</v>
       </c>
       <c r="H14" s="31"/>
       <c r="I14" s="33">
         <f t="shared" si="3"/>
-        <v>0.8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -37396,12 +37417,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D16" s="57">
-        <v>7.4999999999999991</v>
+        <f>SUM(D9:D15)</f>
+        <v>26.8</v>
       </c>
       <c r="E16" s="26"/>
       <c r="I16" s="27">
         <f>SUM(I9:I15)</f>
-        <v>7.6999999999999993</v>
+        <v>26.8</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -37429,7 +37451,7 @@
         <v>2389</v>
       </c>
       <c r="D19" s="55">
-        <v>0.9</v>
+        <v>40</v>
       </c>
       <c r="E19" s="40"/>
       <c r="F19" s="47">
@@ -37437,12 +37459,12 @@
       </c>
       <c r="G19" s="48">
         <f t="shared" ref="G19:G22" si="4">D19/F19</f>
-        <v>0.9</v>
+        <v>40</v>
       </c>
       <c r="H19" s="34"/>
       <c r="I19" s="33">
         <f>F19*G19</f>
-        <v>0.9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -37527,7 +37549,7 @@
       <c r="E23" s="27"/>
       <c r="I23" s="27">
         <f>SUM(I19:I22)</f>
-        <v>14.700000000000001</v>
+        <v>53.800000000000004</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -37557,7 +37579,7 @@
         <v>24</v>
       </c>
       <c r="D26" s="55">
-        <v>1.5</v>
+        <v>30</v>
       </c>
       <c r="E26" s="40"/>
       <c r="F26" s="47">
@@ -37565,12 +37587,12 @@
       </c>
       <c r="G26" s="48">
         <f t="shared" ref="G26:G31" si="6">D26/F26</f>
-        <v>1.5</v>
+        <v>30</v>
       </c>
       <c r="H26" s="34"/>
       <c r="I26" s="33">
         <f>F26*G26</f>
-        <v>1.5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -37705,7 +37727,7 @@
       <c r="E32" s="27"/>
       <c r="I32" s="27">
         <f>SUM(I26:I31)</f>
-        <v>13.9</v>
+        <v>42.4</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -38030,7 +38052,7 @@
       <c r="H50" s="27"/>
       <c r="I50" s="27">
         <f>I6+I16+I23+I32+I40+I48+I32</f>
-        <v>130</v>
+        <v>245.20000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -38158,4 +38180,633 @@
   <pageMargins left="0.45" right="0.45" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="69" fitToHeight="2" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>2355</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>2356</v>
+      </c>
+      <c r="D1" s="69" t="s">
+        <v>2357</v>
+      </c>
+      <c r="E1" s="69" t="s">
+        <v>2358</v>
+      </c>
+      <c r="F1" s="69" t="s">
+        <v>2359</v>
+      </c>
+      <c r="G1" s="69" t="s">
+        <v>2360</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17">
+        <v>25</v>
+      </c>
+      <c r="C2" s="17">
+        <v>73</v>
+      </c>
+      <c r="D2" s="17">
+        <v>185</v>
+      </c>
+      <c r="E2" s="17">
+        <v>57</v>
+      </c>
+      <c r="F2" s="17">
+        <v>61</v>
+      </c>
+      <c r="G2" s="17">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17">
+        <v>46</v>
+      </c>
+      <c r="C3" s="17">
+        <v>67</v>
+      </c>
+      <c r="D3" s="17">
+        <v>39</v>
+      </c>
+      <c r="E3" s="17">
+        <v>55</v>
+      </c>
+      <c r="F3" s="17">
+        <v>12</v>
+      </c>
+      <c r="G3" s="17">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17">
+        <v>29</v>
+      </c>
+      <c r="C4" s="17">
+        <v>14</v>
+      </c>
+      <c r="D4" s="17">
+        <v>13</v>
+      </c>
+      <c r="E4" s="17">
+        <v>96</v>
+      </c>
+      <c r="F4" s="17">
+        <v>17</v>
+      </c>
+      <c r="G4" s="17">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="17">
+        <v>78</v>
+      </c>
+      <c r="C5" s="17">
+        <v>93</v>
+      </c>
+      <c r="D5" s="17">
+        <v>59</v>
+      </c>
+      <c r="E5" s="17">
+        <v>86</v>
+      </c>
+      <c r="F5" s="17">
+        <v>62</v>
+      </c>
+      <c r="G5" s="17">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="17">
+        <v>81</v>
+      </c>
+      <c r="C6" s="17">
+        <v>66</v>
+      </c>
+      <c r="D6" s="17">
+        <v>59</v>
+      </c>
+      <c r="E6" s="17">
+        <v>10</v>
+      </c>
+      <c r="F6" s="17">
+        <v>99</v>
+      </c>
+      <c r="G6" s="17">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="17">
+        <v>71</v>
+      </c>
+      <c r="C7" s="17">
+        <v>35</v>
+      </c>
+      <c r="D7" s="17">
+        <v>88</v>
+      </c>
+      <c r="E7" s="17">
+        <v>49</v>
+      </c>
+      <c r="F7" s="17">
+        <v>30</v>
+      </c>
+      <c r="G7" s="17">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="17">
+        <v>23</v>
+      </c>
+      <c r="C8" s="17">
+        <v>40</v>
+      </c>
+      <c r="D8" s="17">
+        <v>47</v>
+      </c>
+      <c r="E8" s="17">
+        <v>98</v>
+      </c>
+      <c r="F8" s="17">
+        <v>37</v>
+      </c>
+      <c r="G8" s="17">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="17">
+        <v>31</v>
+      </c>
+      <c r="C9" s="17">
+        <v>59</v>
+      </c>
+      <c r="D9" s="17">
+        <v>92</v>
+      </c>
+      <c r="E9" s="17">
+        <v>74</v>
+      </c>
+      <c r="F9" s="17">
+        <v>91</v>
+      </c>
+      <c r="G9" s="17">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="17">
+        <v>36</v>
+      </c>
+      <c r="C10" s="17">
+        <v>52</v>
+      </c>
+      <c r="D10" s="17">
+        <v>65</v>
+      </c>
+      <c r="E10" s="17">
+        <v>41</v>
+      </c>
+      <c r="F10" s="17">
+        <v>45</v>
+      </c>
+      <c r="G10" s="17">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="17">
+        <v>28</v>
+      </c>
+      <c r="C11" s="17">
+        <v>2</v>
+      </c>
+      <c r="D11" s="17">
+        <v>76</v>
+      </c>
+      <c r="E11" s="17">
+        <v>68</v>
+      </c>
+      <c r="F11" s="17">
+        <v>69</v>
+      </c>
+      <c r="G11" s="17">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7">
+        <v>5</v>
+      </c>
+      <c r="C12" s="8">
+        <v>2</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1</v>
+      </c>
+      <c r="G12" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10">
+        <f t="shared" ref="B13:F13" si="0">SUM(B2:B12)</f>
+        <v>453</v>
+      </c>
+      <c r="C13" s="10">
+        <f t="shared" si="0"/>
+        <v>503</v>
+      </c>
+      <c r="D13" s="10">
+        <f t="shared" si="0"/>
+        <v>723</v>
+      </c>
+      <c r="E13" s="10">
+        <f t="shared" si="0"/>
+        <v>634</v>
+      </c>
+      <c r="F13" s="10">
+        <f t="shared" si="0"/>
+        <v>524</v>
+      </c>
+      <c r="G13" s="10">
+        <f>SUM(G2:G12) +G10</f>
+        <v>744</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="69" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C16" s="69" t="s">
+        <v>2362</v>
+      </c>
+      <c r="D16" s="69" t="s">
+        <v>2363</v>
+      </c>
+      <c r="E16" s="69" t="s">
+        <v>2365</v>
+      </c>
+      <c r="F16" s="69" t="s">
+        <v>2366</v>
+      </c>
+      <c r="G16" s="69" t="s">
+        <v>2367</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="17">
+        <v>69</v>
+      </c>
+      <c r="C17" s="17">
+        <v>63</v>
+      </c>
+      <c r="D17" s="17">
+        <v>59</v>
+      </c>
+      <c r="E17" s="73">
+        <v>78</v>
+      </c>
+      <c r="F17" s="73">
+        <v>95</v>
+      </c>
+      <c r="G17" s="73">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="17">
+        <v>97</v>
+      </c>
+      <c r="C18" s="17">
+        <v>21</v>
+      </c>
+      <c r="D18" s="17">
+        <v>18</v>
+      </c>
+      <c r="E18" s="73">
+        <v>81</v>
+      </c>
+      <c r="F18" s="73">
+        <v>89</v>
+      </c>
+      <c r="G18" s="73">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="17">
+        <v>16</v>
+      </c>
+      <c r="C19" s="17">
+        <v>38</v>
+      </c>
+      <c r="D19" s="17">
+        <v>24</v>
+      </c>
+      <c r="E19" s="73">
+        <v>71</v>
+      </c>
+      <c r="F19" s="73">
+        <v>79</v>
+      </c>
+      <c r="G19" s="73">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="17">
+        <v>11</v>
+      </c>
+      <c r="C20" s="17">
+        <v>129</v>
+      </c>
+      <c r="D20" s="17">
+        <v>100</v>
+      </c>
+      <c r="E20" s="73">
+        <v>29</v>
+      </c>
+      <c r="F20" s="73">
+        <v>25</v>
+      </c>
+      <c r="G20" s="73">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="17">
+        <v>94</v>
+      </c>
+      <c r="C21" s="17">
+        <v>64</v>
+      </c>
+      <c r="D21" s="17">
+        <v>56</v>
+      </c>
+      <c r="E21" s="73">
+        <v>22</v>
+      </c>
+      <c r="F21" s="73">
+        <v>80</v>
+      </c>
+      <c r="G21" s="73">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="17">
+        <v>79</v>
+      </c>
+      <c r="C22" s="17">
+        <v>33</v>
+      </c>
+      <c r="D22" s="17">
+        <v>72</v>
+      </c>
+      <c r="E22" s="73">
+        <v>20</v>
+      </c>
+      <c r="F22" s="73">
+        <v>19</v>
+      </c>
+      <c r="G22" s="73">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="17">
+        <v>87</v>
+      </c>
+      <c r="C23" s="17">
+        <v>60</v>
+      </c>
+      <c r="D23" s="17">
+        <v>34</v>
+      </c>
+      <c r="E23" s="73">
+        <v>46</v>
+      </c>
+      <c r="F23" s="73">
+        <v>55</v>
+      </c>
+      <c r="G23" s="73">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="17">
+        <v>51</v>
+      </c>
+      <c r="C24" s="17">
+        <v>54</v>
+      </c>
+      <c r="D24" s="17">
+        <v>44</v>
+      </c>
+      <c r="E24" s="73">
+        <v>23</v>
+      </c>
+      <c r="F24" s="73">
+        <v>33</v>
+      </c>
+      <c r="G24" s="73">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="17">
+        <v>75</v>
+      </c>
+      <c r="C25" s="17">
+        <v>6</v>
+      </c>
+      <c r="D25" s="17">
+        <v>69</v>
+      </c>
+      <c r="E25" s="73">
+        <v>31</v>
+      </c>
+      <c r="F25" s="73">
+        <v>110</v>
+      </c>
+      <c r="G25" s="73">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="17">
+        <v>70</v>
+      </c>
+      <c r="C26" s="17">
+        <v>8</v>
+      </c>
+      <c r="D26" s="17">
+        <v>50</v>
+      </c>
+      <c r="E26" s="73">
+        <v>36</v>
+      </c>
+      <c r="F26" s="73">
+        <v>33</v>
+      </c>
+      <c r="G26" s="73">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="7">
+        <v>3</v>
+      </c>
+      <c r="C27" s="9">
+        <v>1</v>
+      </c>
+      <c r="D27" s="9">
+        <v>159</v>
+      </c>
+      <c r="E27" s="9">
+        <v>2</v>
+      </c>
+      <c r="F27" s="9">
+        <v>2</v>
+      </c>
+      <c r="G27" s="9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="10">
+        <f>SUM(B21:B27)</f>
+        <v>459</v>
+      </c>
+      <c r="C28" s="10">
+        <f>SUM(C21:C27)</f>
+        <v>226</v>
+      </c>
+      <c r="D28" s="10">
+        <f>SUM(D21:D27)</f>
+        <v>484</v>
+      </c>
+      <c r="E28" s="10">
+        <f>SUM(E21:E27)</f>
+        <v>180</v>
+      </c>
+      <c r="F28" s="10">
+        <f>SUM(F21:F27)</f>
+        <v>332</v>
+      </c>
+      <c r="G28" s="11">
+        <f>SUM(G21:G27)</f>
+        <v>330</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update image to include NA
</commit_message>
<xml_diff>
--- a/data/MockData.xlsx
+++ b/data/MockData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6324" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6324" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="7" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Peremptory_modified" sheetId="4" r:id="rId5"/>
     <sheet name="Template" sheetId="3" r:id="rId6"/>
     <sheet name="CourtB-Filing" sheetId="8" r:id="rId7"/>
+    <sheet name="CourtC-Filing" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5045" uniqueCount="2405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5081" uniqueCount="2407">
   <si>
     <t>Case Type</t>
   </si>
@@ -7433,6 +7435,12 @@
   </si>
   <si>
     <t>Case Initiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mental Health </t>
+  </si>
+  <si>
+    <t>Mental Health</t>
   </si>
 </sst>
 </file>
@@ -8054,6 +8062,12 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -8065,12 +8079,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -8658,24 +8666,24 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="76">
+      <c r="B1" s="78">
         <v>2016</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="76">
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="78">
         <v>2017</v>
       </c>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="74" t="s">
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="76" t="s">
         <v>76</v>
       </c>
     </row>
@@ -8722,7 +8730,7 @@
       <c r="N2" s="69" t="s">
         <v>2367</v>
       </c>
-      <c r="O2" s="75"/>
+      <c r="O2" s="77"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -38186,8 +38194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="A1:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38593,7 +38601,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="79" t="s">
+      <c r="A20" s="75" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="17">
@@ -38616,7 +38624,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="78" t="s">
+      <c r="A21" s="74" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="17">
@@ -38781,27 +38789,27 @@
         <v>12</v>
       </c>
       <c r="B28" s="10">
-        <f>SUM(B21:B27)</f>
+        <f t="shared" ref="B28:G28" si="1">SUM(B21:B27)</f>
         <v>459</v>
       </c>
       <c r="C28" s="10">
-        <f>SUM(C21:C27)</f>
+        <f t="shared" si="1"/>
         <v>226</v>
       </c>
       <c r="D28" s="10">
-        <f>SUM(D21:D27)</f>
+        <f t="shared" si="1"/>
         <v>484</v>
       </c>
       <c r="E28" s="10">
-        <f>SUM(E21:E27)</f>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="F28" s="10">
-        <f>SUM(F21:F27)</f>
+        <f t="shared" si="1"/>
         <v>332</v>
       </c>
       <c r="G28" s="11">
-        <f>SUM(G21:G27)</f>
+        <f t="shared" si="1"/>
         <v>330</v>
       </c>
     </row>
@@ -38809,4 +38817,625 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>2357</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>2358</v>
+      </c>
+      <c r="D1" s="69" t="s">
+        <v>2359</v>
+      </c>
+      <c r="E1" s="69" t="s">
+        <v>2355</v>
+      </c>
+      <c r="F1" s="69" t="s">
+        <v>2356</v>
+      </c>
+      <c r="G1" s="69" t="s">
+        <v>2360</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17">
+        <v>185</v>
+      </c>
+      <c r="C2" s="17">
+        <v>57</v>
+      </c>
+      <c r="D2" s="17">
+        <v>61</v>
+      </c>
+      <c r="E2" s="17">
+        <v>25</v>
+      </c>
+      <c r="F2" s="17">
+        <v>10</v>
+      </c>
+      <c r="G2" s="17">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17">
+        <v>39</v>
+      </c>
+      <c r="C3" s="17">
+        <v>55</v>
+      </c>
+      <c r="D3" s="17">
+        <v>64</v>
+      </c>
+      <c r="E3" s="17">
+        <v>46</v>
+      </c>
+      <c r="F3" s="17">
+        <v>67</v>
+      </c>
+      <c r="G3" s="17">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17">
+        <v>50</v>
+      </c>
+      <c r="C4" s="17">
+        <v>96</v>
+      </c>
+      <c r="D4" s="17">
+        <v>129</v>
+      </c>
+      <c r="E4" s="17">
+        <v>29</v>
+      </c>
+      <c r="F4" s="17">
+        <v>14</v>
+      </c>
+      <c r="G4" s="17">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="17">
+        <v>59</v>
+      </c>
+      <c r="C5" s="17">
+        <v>86</v>
+      </c>
+      <c r="D5" s="17">
+        <v>62</v>
+      </c>
+      <c r="E5" s="17">
+        <v>78</v>
+      </c>
+      <c r="F5" s="17">
+        <v>50</v>
+      </c>
+      <c r="G5" s="17">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="17">
+        <v>59</v>
+      </c>
+      <c r="C6" s="17">
+        <v>10</v>
+      </c>
+      <c r="D6" s="17">
+        <v>99</v>
+      </c>
+      <c r="E6" s="17">
+        <v>81</v>
+      </c>
+      <c r="F6" s="17">
+        <v>70</v>
+      </c>
+      <c r="G6" s="17">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="17">
+        <v>88</v>
+      </c>
+      <c r="C7" s="17">
+        <v>49</v>
+      </c>
+      <c r="D7" s="17">
+        <v>30</v>
+      </c>
+      <c r="E7" s="17">
+        <v>80</v>
+      </c>
+      <c r="F7" s="17">
+        <v>60</v>
+      </c>
+      <c r="G7" s="17">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="17">
+        <v>47</v>
+      </c>
+      <c r="C8" s="17">
+        <v>98</v>
+      </c>
+      <c r="D8" s="17">
+        <v>37</v>
+      </c>
+      <c r="E8" s="17">
+        <v>50</v>
+      </c>
+      <c r="F8" s="17">
+        <v>40</v>
+      </c>
+      <c r="G8" s="17">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>2406</v>
+      </c>
+      <c r="B9" s="17">
+        <v>92</v>
+      </c>
+      <c r="C9" s="17">
+        <v>74</v>
+      </c>
+      <c r="D9" s="17">
+        <v>91</v>
+      </c>
+      <c r="E9" s="17">
+        <v>31</v>
+      </c>
+      <c r="F9" s="17">
+        <v>59</v>
+      </c>
+      <c r="G9" s="17">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="17">
+        <v>86</v>
+      </c>
+      <c r="C10" s="17">
+        <v>68</v>
+      </c>
+      <c r="D10" s="17">
+        <v>69</v>
+      </c>
+      <c r="E10" s="17">
+        <v>100</v>
+      </c>
+      <c r="F10" s="17">
+        <v>2</v>
+      </c>
+      <c r="G10" s="17">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0</v>
+      </c>
+      <c r="D11" s="9">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7">
+        <v>5</v>
+      </c>
+      <c r="F11" s="8">
+        <v>2</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="10">
+        <f>SUM(B2:B11)</f>
+        <v>705</v>
+      </c>
+      <c r="C12" s="10">
+        <f>SUM(C2:C11)</f>
+        <v>593</v>
+      </c>
+      <c r="D12" s="10">
+        <f>SUM(D2:D11)</f>
+        <v>643</v>
+      </c>
+      <c r="E12" s="10">
+        <f t="shared" ref="E12:G12" si="0">SUM(E2:E11)</f>
+        <v>525</v>
+      </c>
+      <c r="F12" s="10">
+        <f t="shared" si="0"/>
+        <v>374</v>
+      </c>
+      <c r="G12" s="10">
+        <f t="shared" si="0"/>
+        <v>641</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="69" t="s">
+        <v>2363</v>
+      </c>
+      <c r="C15" s="69" t="s">
+        <v>2365</v>
+      </c>
+      <c r="D15" s="69" t="s">
+        <v>2366</v>
+      </c>
+      <c r="E15" s="69" t="s">
+        <v>2361</v>
+      </c>
+      <c r="F15" s="69" t="s">
+        <v>2362</v>
+      </c>
+      <c r="G15" s="69" t="s">
+        <v>2367</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="17">
+        <v>59</v>
+      </c>
+      <c r="C16" s="73">
+        <v>78</v>
+      </c>
+      <c r="D16" s="73">
+        <v>95</v>
+      </c>
+      <c r="E16" s="17">
+        <v>69</v>
+      </c>
+      <c r="F16" s="17">
+        <v>63</v>
+      </c>
+      <c r="G16" s="73">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="17">
+        <v>81</v>
+      </c>
+      <c r="C17" s="73">
+        <v>81</v>
+      </c>
+      <c r="D17" s="73">
+        <v>89</v>
+      </c>
+      <c r="E17" s="17">
+        <v>97</v>
+      </c>
+      <c r="F17" s="17">
+        <v>60</v>
+      </c>
+      <c r="G17" s="73">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="17">
+        <v>24</v>
+      </c>
+      <c r="C18" s="73">
+        <v>71</v>
+      </c>
+      <c r="D18" s="73">
+        <v>79</v>
+      </c>
+      <c r="E18" s="17">
+        <v>16</v>
+      </c>
+      <c r="F18" s="17">
+        <v>38</v>
+      </c>
+      <c r="G18" s="73">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="75" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="17">
+        <v>100</v>
+      </c>
+      <c r="C19" s="73">
+        <v>29</v>
+      </c>
+      <c r="D19" s="73">
+        <v>25</v>
+      </c>
+      <c r="E19" s="17">
+        <v>0</v>
+      </c>
+      <c r="F19" s="17">
+        <v>129</v>
+      </c>
+      <c r="G19" s="73">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="17">
+        <v>56</v>
+      </c>
+      <c r="C20" s="73">
+        <v>22</v>
+      </c>
+      <c r="D20" s="73">
+        <v>80</v>
+      </c>
+      <c r="E20" s="17">
+        <v>94</v>
+      </c>
+      <c r="F20" s="17">
+        <v>64</v>
+      </c>
+      <c r="G20" s="73">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="17">
+        <v>72</v>
+      </c>
+      <c r="C21" s="73">
+        <v>20</v>
+      </c>
+      <c r="D21" s="73">
+        <v>19</v>
+      </c>
+      <c r="E21" s="17">
+        <v>79</v>
+      </c>
+      <c r="F21" s="17">
+        <v>33</v>
+      </c>
+      <c r="G21" s="73">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="17">
+        <v>90</v>
+      </c>
+      <c r="C22" s="73">
+        <v>50</v>
+      </c>
+      <c r="D22" s="73">
+        <v>55</v>
+      </c>
+      <c r="E22" s="17">
+        <v>150</v>
+      </c>
+      <c r="F22" s="17">
+        <v>120</v>
+      </c>
+      <c r="G22" s="73">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>2405</v>
+      </c>
+      <c r="B23" s="17">
+        <v>44</v>
+      </c>
+      <c r="C23" s="73">
+        <v>23</v>
+      </c>
+      <c r="D23" s="73">
+        <v>33</v>
+      </c>
+      <c r="E23" s="17">
+        <v>51</v>
+      </c>
+      <c r="F23" s="17">
+        <v>54</v>
+      </c>
+      <c r="G23" s="73">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="17">
+        <v>1</v>
+      </c>
+      <c r="C24" s="73">
+        <v>36</v>
+      </c>
+      <c r="D24" s="73">
+        <v>78</v>
+      </c>
+      <c r="E24" s="17">
+        <v>70</v>
+      </c>
+      <c r="F24" s="17">
+        <v>80</v>
+      </c>
+      <c r="G24" s="73">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="9">
+        <v>159</v>
+      </c>
+      <c r="C25" s="9">
+        <v>2</v>
+      </c>
+      <c r="D25" s="9">
+        <v>2</v>
+      </c>
+      <c r="E25" s="7">
+        <v>3</v>
+      </c>
+      <c r="F25" s="9">
+        <v>1</v>
+      </c>
+      <c r="G25" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="10">
+        <f>SUM(B20:B25)</f>
+        <v>422</v>
+      </c>
+      <c r="C26" s="10">
+        <f>SUM(C20:C25)</f>
+        <v>153</v>
+      </c>
+      <c r="D26" s="10">
+        <f>SUM(D20:D25)</f>
+        <v>267</v>
+      </c>
+      <c r="E26" s="10">
+        <f t="shared" ref="E26:G26" si="1">SUM(E20:E25)</f>
+        <v>447</v>
+      </c>
+      <c r="F26" s="10">
+        <f t="shared" si="1"/>
+        <v>352</v>
+      </c>
+      <c r="G26" s="11">
+        <f t="shared" si="1"/>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add new data for string lesson
</commit_message>
<xml_diff>
--- a/data/MockData.xlsx
+++ b/data/MockData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6324" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6324" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="7" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Template" sheetId="3" r:id="rId6"/>
     <sheet name="CourtB-Filing" sheetId="8" r:id="rId7"/>
     <sheet name="CourtC-Filing" sheetId="9" r:id="rId8"/>
-    <sheet name="Sheet2" sheetId="10" r:id="rId9"/>
+    <sheet name="Address" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5081" uniqueCount="2407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5094" uniqueCount="2414">
   <si>
     <t>Case Type</t>
   </si>
@@ -7441,6 +7441,27 @@
   </si>
   <si>
     <t>Mental Health</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>2120 Martin Luther King Jr. Way,</t>
+  </si>
+  <si>
+    <t>1221 Oak Street,</t>
+  </si>
+  <si>
+    <t>1225 Fallon Street,</t>
+  </si>
+  <si>
+    <t>24405 Amador Street</t>
+  </si>
+  <si>
+    <t>661 Washington Street,</t>
+  </si>
+  <si>
+    <t>2500 Fairmont Drive, Suite 3013</t>
   </si>
 </sst>
 </file>
@@ -38823,7 +38844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -39430,12 +39451,83 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2407</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>2408</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>2409</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>2410</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>2411</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>2412</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>2412</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>2413</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>2409</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>2411</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>2410</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>2410</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
+        <v>2411</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>